<commit_message>
Daily II - poprawka
Poprawiona wersja dokumentu z opisem pracy przy FEAT
</commit_message>
<xml_diff>
--- a/etap_drugi/Daily - II (1).xlsx
+++ b/etap_drugi/Daily - II (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ewa\Desktop\Studia\Inzynieria oprogramowania\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38503DA6-7021-4607-9EBE-DD9092208DE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B7A8C5-5EE0-4CF1-9A2A-B3B2CF577161}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="1308" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Co zrobiłam/em?</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Kamil Sajdak</t>
   </si>
   <si>
-    <t>Sprawdzenie poprawności cech FEAT</t>
-  </si>
-  <si>
     <t>Karty CRC - czy tylko ze słownika, który bazował na wymaganiach zamawiającego, czy może też na wizji systemu (tam dużo dodatkowych klas chyba zostanie dodanych). Co do TERM to czy powinno być może jeszcze więcej (wydaje mi się że nie, ale może trzeba też tłumaczyć dane które wprowadzamy).</t>
   </si>
   <si>
@@ -100,6 +97,12 @@
   </si>
   <si>
     <t>Szczegółowość wymagań STRQ - czy ma być podział  na konkretne role ?</t>
+  </si>
+  <si>
+    <t>Naniesienie poprawek do dokumentu z cechami systemu FEAT, dodanie kilku nowych cech.</t>
+  </si>
+  <si>
+    <t>Przeanalizowanie dokumentów w poszukiwaniu nowych cech systemu.</t>
   </si>
 </sst>
 </file>
@@ -164,12 +167,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -525,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -533,13 +536,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -547,27 +550,27 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +588,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -635,32 +638,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>